<commit_message>
Baselined from internal Repository last_commit:a99de9db7e0c3e23ffc1e4e34dad7b187f4ccebc
</commit_message>
<xml_diff>
--- a/meetings.xlsx
+++ b/meetings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramrenne/Documents/Documents/cases/Webex_Meetings_Creation_Integration/meetings/gve_devnet_webex_meetings_creation_integration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramrenne/Documents/Documents/cases/Webex_Meetings_Creation_Integration/renaming/gve_devnet_webex_meetings_creation_integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C903189C-61B8-1F40-B828-EA9EA4C9C14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217D712E-5212-4046-940A-79A528E7FF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11080" yWindow="-21100" windowWidth="27320" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>